<commit_message>
original excel for education
</commit_message>
<xml_diff>
--- a/xj/Educational Attainment.xlsx
+++ b/xj/Educational Attainment.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Home\SHARED\DIGEST\19 Digest\022119\Drafts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuejin/Desktop/CUMC_semester1/Courses/Data Science/homework/life_saver.github.io/xj/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE60F163-1636-F44D-B842-A4D676740C3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="19200" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Educational Attainment" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Wyoming</t>
   </si>
@@ -208,27 +209,30 @@
   </si>
   <si>
     <t>Data is from 2000 Census and five-year ACS estimates for 2008-2012 and 2013-2017</t>
+  </si>
+  <si>
+    <t>https://ssti.org/blog/useful-stats-educational-attainment-across-states-2000-2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -236,8 +240,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -319,9 +330,9 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -341,10 +352,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -352,8 +363,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -630,49 +641,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="12">
+      <c r="B1" s="11">
         <v>2000</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="12">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="11">
         <v>2012</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="12">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="11">
         <v>2017</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="10"/>
-    </row>
-    <row r="2" spans="1:19" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" s="5" customFormat="1" ht="47.25" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>58</v>
       </c>
@@ -731,7 +742,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
@@ -790,7 +801,7 @@
         <v>0.45583627359393181</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -849,7 +860,7 @@
         <v>0.3522406518565882</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
@@ -908,7 +919,7 @@
         <v>0.37664350916428174</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
@@ -967,7 +978,7 @@
         <v>0.48726841477109634</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
@@ -1026,7 +1037,7 @@
         <v>0.38106976049849373</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
@@ -1085,7 +1096,7 @@
         <v>0.30440479795838982</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1144,7 +1155,7 @@
         <v>0.36934367134258517</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -1203,7 +1214,7 @@
         <v>0.41866807870583539</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
@@ -1262,7 +1273,7 @@
         <v>0.27334501080898954</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -1321,7 +1332,7 @@
         <v>0.41385028382059375</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1380,7 +1391,7 @@
         <v>0.41782815985954819</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
@@ -1439,7 +1450,7 @@
         <v>0.36128697984395319</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1509,7 @@
         <v>0.37181279117029453</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -1557,7 +1568,7 @@
         <v>0.37767345531929725</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
@@ -1616,7 +1627,7 @@
         <v>0.45444267483489342</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -1675,7 +1686,7 @@
         <v>0.3967258793160644</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
@@ -1734,7 +1745,7 @@
         <v>0.35726260255117159</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -1793,7 +1804,7 @@
         <v>0.47892990386775963</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1852,7 +1863,7 @@
         <v>0.4954967046336935</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1922,7 @@
         <v>0.4019952428814903</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
@@ -1970,7 +1981,7 @@
         <v>0.35291167441148386</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
@@ -2029,7 +2040,7 @@
         <v>0.34436430529799411</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
@@ -2088,7 +2099,7 @@
         <v>0.39029820362346745</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -2147,7 +2158,7 @@
         <v>0.32604049364557719</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -2206,7 +2217,7 @@
         <v>0.4700258319994724</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
@@ -2265,7 +2276,7 @@
         <v>0.41737043160482795</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -2324,7 +2335,7 @@
         <v>0.36334720330037973</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
@@ -2383,7 +2394,7 @@
         <v>0.35790482087657899</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -2442,7 +2453,7 @@
         <v>0.42462359433807428</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>0.35144139627513782</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
@@ -2560,7 +2571,7 @@
         <v>0.38765342045417855</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
@@ -2619,7 +2630,7 @@
         <v>0.41436636436672625</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35" s="4" t="s">
         <v>19</v>
       </c>
@@ -2678,7 +2689,7 @@
         <v>0.4016399028783727</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -2737,7 +2748,7 @@
         <v>0.39230795536824031</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" s="4" t="s">
         <v>17</v>
       </c>
@@ -2796,7 +2807,7 @@
         <v>0.34833879173618404</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -2855,7 +2866,7 @@
         <v>0.43765027287767094</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
@@ -2914,7 +2925,7 @@
         <v>0.43955875257686738</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
@@ -2973,7 +2984,7 @@
         <v>0.33224789694465917</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19">
       <c r="A41" s="4" t="s">
         <v>13</v>
       </c>
@@ -3032,7 +3043,7 @@
         <v>0.45698733720513712</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19">
       <c r="A42" s="4" t="s">
         <v>12</v>
       </c>
@@ -3091,7 +3102,7 @@
         <v>0.52910731218245344</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19">
       <c r="A43" s="4" t="s">
         <v>11</v>
       </c>
@@ -3150,7 +3161,7 @@
         <v>0.40550091119640291</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19">
       <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
@@ -3209,7 +3220,7 @@
         <v>0.42879377291503101</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19">
       <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
@@ -3268,7 +3279,7 @@
         <v>0.39055306320849797</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -3327,7 +3338,7 @@
         <v>0.4610720226864205</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19">
       <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
@@ -3386,7 +3397,7 @@
         <v>0.42271982398051244</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19">
       <c r="A48" s="4" t="s">
         <v>6</v>
       </c>
@@ -3445,7 +3456,7 @@
         <v>0.31052785570452474</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19">
       <c r="A49" s="4" t="s">
         <v>5</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>0.37313085179264671</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" s="4" t="s">
         <v>4</v>
       </c>
@@ -3563,7 +3574,7 @@
         <v>0.35253614610004108</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="4" t="s">
         <v>3</v>
       </c>
@@ -3622,7 +3633,7 @@
         <v>0.31667577263735802</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="4" t="s">
         <v>2</v>
       </c>
@@ -3681,7 +3692,7 @@
         <v>0.54634236838748829</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19">
       <c r="A53" s="4" t="s">
         <v>1</v>
       </c>
@@ -3740,7 +3751,7 @@
         <v>0.39576837804031717</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" s="4" t="s">
         <v>0</v>
       </c>
@@ -3805,26 +3816,33 @@
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>